<commit_message>
Added VWAP excel and Venue market data test
</commit_message>
<xml_diff>
--- a/VWAP test.xlsx
+++ b/VWAP test.xlsx
@@ -349,52 +349,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:D7"/>
+  <dimension ref="C3:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>1000000</v>
       </c>
       <c r="D3">
         <v>1.0900000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f>C3*D3</f>
+        <v>1090000</v>
+      </c>
+      <c r="G3">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="H3">
+        <f>C3*G3</f>
+        <v>1090000</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>2000000</v>
       </c>
       <c r="D4">
         <v>1.089</v>
       </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f t="shared" ref="E4:E7" si="0">C4*D4</f>
+        <v>2178000</v>
+      </c>
+      <c r="G4">
+        <v>1.091</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H7" si="1">C4*G4</f>
+        <v>2182000</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>5000000</v>
       </c>
       <c r="D5">
         <v>1.0880000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>5440000</v>
+      </c>
+      <c r="G5">
+        <v>1.0920000000000001</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>5460000</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>10000000</v>
       </c>
       <c r="D6">
         <v>1.087</v>
       </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>10870000</v>
+      </c>
+      <c r="G6">
+        <v>1.093</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>10930000</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>20000000</v>
       </c>
       <c r="D7">
         <v>1.0860000000000001</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>21720000</v>
+      </c>
+      <c r="G7">
+        <v>1.0940000000000001</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>21880000</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <f>SUM(C3:C8)</f>
+        <v>38000000</v>
+      </c>
+      <c r="E9">
+        <f>SUM(E3:E8)</f>
+        <v>41298000</v>
+      </c>
+      <c r="H9">
+        <f>SUM(H3:H8)</f>
+        <v>41542000</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f>E9/C9</f>
+        <v>1.0867894736842105</v>
+      </c>
+      <c r="G11">
+        <f>H9/C9</f>
+        <v>1.0932105263157894</v>
       </c>
     </row>
   </sheetData>

</xml_diff>